<commit_message>
SA & SD File Upload
</commit_message>
<xml_diff>
--- a/戶政找收系統文件/文件/內部/Table Schema.xlsx
+++ b/戶政找收系統文件/文件/內部/Table Schema.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="共用" sheetId="1" r:id="rId1"/>
     <sheet name="基礎資料" sheetId="2" r:id="rId2"/>
+    <sheet name="交易紀錄" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="190">
   <si>
     <t>參數檔</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,6 +276,157 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費項目名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>項目描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費群組</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費科目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>過帳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>過帳日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紀錄時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DateField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PenaltyID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PenaltyName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ColseDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecordTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能圖示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MenuParent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MenuIcon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BooleanField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CharField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Penalty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Term</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null=True</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>default=''</t>
+  </si>
+  <si>
+    <t>auto_now=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForeignKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auth_user</t>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unique=True</t>
+  </si>
+  <si>
     <t>條款編號</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -287,23 +439,213 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費項目名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費金額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>項目描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費群組</t>
+    <t>TermID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TermName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證庫存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvoiceNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_FeeItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Invoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntegerField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_FeeItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_now=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unique=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易紀錄主檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可使用站號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶所代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶所名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站點代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站點名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Store</t>
+  </si>
+  <si>
+    <t>M_Station</t>
+  </si>
+  <si>
+    <t>M_Station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoreID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoreName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StationID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StationName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StationID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -311,31 +653,117 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>收銀人員</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合計金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>付款別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易紀錄明細</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易主檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_FeeItem</t>
+  </si>
+  <si>
     <t>規費科目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>過帳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>過帳日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>紀錄時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DateField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PenaltyID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PenaltyName</t>
+    <t>金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>數量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小計</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否過帳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=False</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BooleanField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_DealMaster</t>
+  </si>
+  <si>
+    <t>M_DealMaster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_DealDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否補登</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DealDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PayType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsCheckout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsOutside</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MasterID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalAmount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -343,107 +771,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TermID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TermName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColseDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecordTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能圖示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MenuParent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MenuIcon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BooleanField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CharField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_Penalty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_Term</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null=True</t>
-  </si>
-  <si>
-    <t>choices</t>
-  </si>
-  <si>
-    <t>default=''</t>
-  </si>
-  <si>
-    <t>auto_now=True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default=True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ForeignKey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>auth_user</t>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unique=True</t>
+    <t>Cashier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_EmployeeCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -785,7 +1118,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -993,7 +1326,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,10 +1340,10 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,15 +1357,15 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F37" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -1041,24 +1374,24 @@
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,7 +1402,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1081,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1097,408 +1430,1058 @@
     <col min="9" max="9" width="11.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" t="s">
+        <v>127</v>
+      </c>
+      <c r="M4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" t="s">
+        <v>149</v>
+      </c>
+      <c r="J24" t="s">
+        <v>142</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" t="s">
+        <v>85</v>
+      </c>
+      <c r="M24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" t="s">
+        <v>150</v>
+      </c>
+      <c r="J25" t="s">
+        <v>143</v>
+      </c>
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K26" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>149</v>
+      </c>
+      <c r="J32" t="s">
+        <v>142</v>
+      </c>
+      <c r="K32" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J33" t="s">
+        <v>144</v>
+      </c>
+      <c r="K33" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" t="s">
+        <v>85</v>
+      </c>
+      <c r="M33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>152</v>
+      </c>
+      <c r="J34" t="s">
+        <v>145</v>
+      </c>
+      <c r="K34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35" t="s">
+        <v>55</v>
+      </c>
+      <c r="K35" t="s">
+        <v>97</v>
+      </c>
+      <c r="L35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="14.75" customWidth="1"/>
+    <col min="12" max="12" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" t="s">
-        <v>105</v>
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" t="s">
+        <v>108</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>129</v>
+      </c>
+      <c r="L3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" t="s">
+        <v>109</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>133</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G5" t="s">
-        <v>105</v>
+        <v>189</v>
+      </c>
+      <c r="H5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" t="s">
+        <v>110</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>127</v>
+      </c>
+      <c r="L5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>101</v>
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I6" t="s">
+        <v>139</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" t="s">
+        <v>111</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" t="s">
+        <v>171</v>
+      </c>
+      <c r="H10" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="I10" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
+      <c r="J10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+      <c r="L10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>54</v>
       </c>
-      <c r="J9" t="s">
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="K9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="J10" t="s">
+      <c r="B14" t="s">
         <v>48</v>
       </c>
-      <c r="K10" t="s">
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="I16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I18" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
         <v>92</v>
       </c>
-      <c r="I19" t="s">
-        <v>82</v>
-      </c>
-      <c r="J19" t="s">
-        <v>74</v>
-      </c>
-      <c r="K19" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E27" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload deal detail table change
</commit_message>
<xml_diff>
--- a/戶政找收系統文件/文件/內部/Table Schema.xlsx
+++ b/戶政找收系統文件/文件/內部/Table Schema.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="206">
   <si>
     <t>參數檔</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -228,587 +228,619 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CardNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否在職</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>異動者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EditDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罰鍰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罰鍰編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罰鍰名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註說明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>條款</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費項目名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>項目描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費群組</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費科目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>過帳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>過帳日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紀錄時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DateField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PenaltyID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PenaltyName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ColseDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecordTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能圖示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MenuParent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MenuIcon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BooleanField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CharField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Penalty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null=True</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>default=''</t>
+  </si>
+  <si>
+    <t>auto_now=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ForeignKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auth_user</t>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unique=True</t>
+  </si>
+  <si>
+    <t>條款編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>條款名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註說明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TermID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TermName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證庫存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvoiceNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_FeeItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Invoice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntegerField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_FeeItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auto_now=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_length=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unique=True</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易紀錄主檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可使用站號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶所代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶所名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站點代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站點名稱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Store</t>
+  </si>
+  <si>
+    <t>M_Station</t>
+  </si>
+  <si>
+    <t>M_Station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoreID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoreName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StationID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StationName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狀態</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收銀人員</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合計金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>付款別</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>憑證號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易紀錄明細</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易主檔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>規費科目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>數量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小計</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否過帳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default=False</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BooleanField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_DealMaster</t>
+  </si>
+  <si>
+    <t>M_DealMaster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_DealDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否補登</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DealDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PayType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsCheckout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsOutside</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MasterID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Qty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cashier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_FeeItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BooleanField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InvoiceNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StationID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立批號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LotNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罰鍰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>條款</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_Term</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FeeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M_EmployeeCard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CharField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>EmployeeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CardNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IsWork</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>是否在職</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Editor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>異動者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EditDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>罰鍰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>罰鍰編號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>罰鍰名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>備註說明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>條款</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費項目名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費金額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>項目描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費群組</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狀態</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費科目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>過帳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>過帳日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>紀錄時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DateField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PenaltyID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PenaltyName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColseDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecordTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能圖示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MenuParent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MenuIcon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BooleanField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CharField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>M_Penalty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TermID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>M_Term</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null=True</t>
-  </si>
-  <si>
-    <t>choices</t>
-  </si>
-  <si>
-    <t>default=''</t>
-  </si>
-  <si>
-    <t>auto_now=True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default=True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ForeignKey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>auth_user</t>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unique=True</t>
-  </si>
-  <si>
-    <t>條款編號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>條款名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>備註說明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TermID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TermName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>憑證號碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用狀態</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用金額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建立者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建立日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Amount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>憑證庫存</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvoiceNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FeeID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FeeName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FeeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FeeID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_FeeItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_Invoice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IntegerField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default=0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_FeeItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>auto_now=True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default=0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max_length=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unique=True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交易紀錄主檔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可使用站號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶所</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>站點</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶所代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶所名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>站點代碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>站點名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_Store</t>
-  </si>
-  <si>
-    <t>M_Station</t>
-  </si>
-  <si>
-    <t>M_Station</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StoreID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StoreName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StationID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StationName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_Store</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>站號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交易日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狀態</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>收銀人員</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合計金額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>付款別</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>憑證號碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交易紀錄明細</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交易主檔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>規費科目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>數量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小計</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>備註</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否過帳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>default=False</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BooleanField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_DealMaster</t>
-  </si>
-  <si>
-    <t>M_DealMaster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_DealDetail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否補登</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DealDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PayType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsCheckout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_Checkout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsOutside</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MasterID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Amount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Qty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalAmount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cashier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_EmployeeCard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M_FeeItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BooleanField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>InvoiceNo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Amount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StationID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Creator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FeeAmount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建立批號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LotNo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1359,7 +1391,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1373,10 +1405,10 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1390,15 +1422,15 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -1407,24 +1439,24 @@
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
         <v>80</v>
       </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>82</v>
-      </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1435,7 +1467,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1450,7 +1482,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1477,10 +1509,10 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1496,56 +1528,56 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="M2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
         <v>14</v>
       </c>
       <c r="L3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -1554,85 +1586,85 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
         <v>121</v>
       </c>
-      <c r="J5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>127</v>
-      </c>
       <c r="M5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I6" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
       </c>
       <c r="L6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="M6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -1641,38 +1673,38 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
+        <v>197</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
         <v>48</v>
@@ -1681,71 +1713,71 @@
         <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J16" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" t="s">
         <v>70</v>
-      </c>
-      <c r="K16" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K17" t="s">
         <v>26</v>
@@ -1753,50 +1785,50 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
@@ -1805,129 +1837,129 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I24" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J24" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K24" t="s">
         <v>14</v>
       </c>
       <c r="L24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="J25" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K25" t="s">
         <v>14</v>
       </c>
       <c r="L25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I27" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
-      </c>
-      <c r="I27" t="s">
-        <v>56</v>
       </c>
       <c r="J27" t="s">
         <v>48</v>
@@ -1936,12 +1968,12 @@
         <v>26</v>
       </c>
       <c r="L27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
@@ -1950,81 +1982,81 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I31" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J32" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L32" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J33" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K33" t="s">
         <v>14</v>
       </c>
       <c r="L33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="K34" t="s">
         <v>14</v>
       </c>
       <c r="L34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K35" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J36" t="s">
         <v>48</v>
@@ -2033,7 +2065,7 @@
         <v>26</v>
       </c>
       <c r="L36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2045,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2067,228 +2099,228 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="I3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="I4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="H5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="I5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="L5" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H6" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="J7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H9" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="I9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J9" t="s">
         <v>26</v>
@@ -2296,48 +2328,45 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
         <v>48</v>
@@ -2346,196 +2375,244 @@
         <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
-        <v>92</v>
+      <c r="E15" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>203</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
         <v>26</v>
       </c>
-      <c r="E27" t="s">
-        <v>92</v>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>